<commit_message>
tests rebuild I need to write how to properly create a game file (. as separator, \n as terminator, etc.)
</commit_message>
<xml_diff>
--- a/docs/tests_index.xlsx
+++ b/docs/tests_index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\repos\games\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ABB7F6-05AA-4D4D-A348-F61CC885C44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82834B7F-F07E-4967-A1CD-473383C16CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B783D0B5-C6EA-4FCF-B986-EFEDF66F7BFD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -51,15 +51,6 @@
     <t>observations</t>
   </si>
   <si>
-    <t>less rows than indicated by row number</t>
-  </si>
-  <si>
-    <t>less words than indicated by word number</t>
-  </si>
-  <si>
-    <t>more words than indicated by word number</t>
-  </si>
-  <si>
     <t>more rows than indicated by row number</t>
   </si>
   <si>
@@ -136,6 +127,42 @@
   </si>
   <si>
     <t>ce_as_024</t>
+  </si>
+  <si>
+    <t>contains null word (length 1)</t>
+  </si>
+  <si>
+    <t>contains null word (length 0)</t>
+  </si>
+  <si>
+    <t>gr_as_001</t>
+  </si>
+  <si>
+    <t>gr_as_002</t>
+  </si>
+  <si>
+    <t>gr_as_003</t>
+  </si>
+  <si>
+    <t>double separator</t>
+  </si>
+  <si>
+    <t>no separator</t>
+  </si>
+  <si>
+    <t>gr_as_004</t>
+  </si>
+  <si>
+    <t>gr_as_005</t>
+  </si>
+  <si>
+    <t>gr_as_006</t>
+  </si>
+  <si>
+    <t>separator different than .</t>
+  </si>
+  <si>
+    <t>row with abnormal length</t>
   </si>
 </sst>
 </file>
@@ -500,9 +527,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C766BE2E-A501-4A19-9656-5430AC1749FA}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -533,146 +560,194 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parser and exception modules created. main module refactored comments in alphasoup
</commit_message>
<xml_diff>
--- a/docs/tests_index.xlsx
+++ b/docs/tests_index.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\repos\games\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82834B7F-F07E-4967-A1CD-473383C16CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538FD61-7B89-48C1-8EF3-A2397C8CB712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B783D0B5-C6EA-4FCF-B986-EFEDF66F7BFD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="alphabet soup" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,25 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>valid</t>
-  </si>
-  <si>
-    <t>expected result</t>
-  </si>
-  <si>
-    <t>observations</t>
-  </si>
-  <si>
-    <t>more rows than indicated by row number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>no</t>
   </si>
@@ -129,9 +111,6 @@
     <t>ce_as_024</t>
   </si>
   <si>
-    <t>contains null word (length 1)</t>
-  </si>
-  <si>
     <t>contains null word (length 0)</t>
   </si>
   <si>
@@ -163,13 +142,46 @@
   </si>
   <si>
     <t>row with abnormal length</t>
+  </si>
+  <si>
+    <t>missed separator</t>
+  </si>
+  <si>
+    <t>Search words must be at least two letters long.</t>
+  </si>
+  <si>
+    <t>missing separator means that parser will fill the wordlist until it reaches a null line ('' has length &lt; 2)</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>VALIDITY</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>EXPECTED RESULT</t>
+  </si>
+  <si>
+    <t>OBSERVATIONS</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>valid game file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,8 +195,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,12 +213,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -206,13 +232,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,231 +586,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C766BE2E-A501-4A19-9656-5430AC1749FA}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="1"/>
-    <col min="3" max="3" width="33.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="11.5546875" style="5"/>
+    <col min="2" max="2" width="11.5546875" style="6"/>
+    <col min="3" max="3" width="33.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="39.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.44140625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
alphasoup commented and fixed so there is not loss of information when looking for directions tests added new module to play (execute.py)
</commit_message>
<xml_diff>
--- a/docs/tests_index.xlsx
+++ b/docs/tests_index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\repos\games\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538FD61-7B89-48C1-8EF3-A2397C8CB712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A133463A-B401-49D3-A2D1-7D027ED513E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B783D0B5-C6EA-4FCF-B986-EFEDF66F7BFD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17592" windowHeight="11652" xr2:uid="{B783D0B5-C6EA-4FCF-B986-EFEDF66F7BFD}"/>
   </bookViews>
   <sheets>
     <sheet name="alphabet soup" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>no</t>
   </si>
@@ -175,6 +175,24 @@
   </si>
   <si>
     <t>valid game file</t>
+  </si>
+  <si>
+    <t>contains null word (length 1)</t>
+  </si>
+  <si>
+    <t>Incorrect table format.</t>
+  </si>
+  <si>
+    <t>Incorrect format. Game file corrupted.</t>
+  </si>
+  <si>
+    <t>non alphabetical characters in table</t>
+  </si>
+  <si>
+    <t>non alphabetical characters in wordlist</t>
+  </si>
+  <si>
+    <t>['Palabra AIRE encontrada entre (0, 0) y (3, 3).', 'Palabra AGUA encontrada entre (0, 0) y (0, 3).', 'Palabra TIERRA no encontrada.', 'Palabra NIU encontrada entre (2, 0) y (0, 2).']</t>
   </si>
 </sst>
 </file>
@@ -629,7 +647,9 @@
       <c r="C2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -640,7 +660,7 @@
         <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>37</v>
@@ -672,7 +692,9 @@
       <c r="C5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -696,18 +718,30 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added grammar tests and derivation tree improved alphasoup
</commit_message>
<xml_diff>
--- a/docs/tests_index.xlsx
+++ b/docs/tests_index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\repos\games\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A133463A-B401-49D3-A2D1-7D027ED513E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58BCA60-2FDE-479D-9CBA-B37988417E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17592" windowHeight="11652" xr2:uid="{B783D0B5-C6EA-4FCF-B986-EFEDF66F7BFD}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
-  <si>
-    <t>no</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>ce_as_001</t>
   </si>
@@ -66,51 +63,6 @@
     <t>ce_as_009</t>
   </si>
   <si>
-    <t>ce_as_010</t>
-  </si>
-  <si>
-    <t>ce_as_011</t>
-  </si>
-  <si>
-    <t>ce_as_012</t>
-  </si>
-  <si>
-    <t>ce_as_013</t>
-  </si>
-  <si>
-    <t>ce_as_014</t>
-  </si>
-  <si>
-    <t>ce_as_015</t>
-  </si>
-  <si>
-    <t>ce_as_016</t>
-  </si>
-  <si>
-    <t>ce_as_017</t>
-  </si>
-  <si>
-    <t>ce_as_018</t>
-  </si>
-  <si>
-    <t>ce_as_019</t>
-  </si>
-  <si>
-    <t>ce_as_020</t>
-  </si>
-  <si>
-    <t>ce_as_021</t>
-  </si>
-  <si>
-    <t>ce_as_022</t>
-  </si>
-  <si>
-    <t>ce_as_023</t>
-  </si>
-  <si>
-    <t>ce_as_024</t>
-  </si>
-  <si>
     <t>contains null word (length 0)</t>
   </si>
   <si>
@@ -123,12 +75,6 @@
     <t>gr_as_003</t>
   </si>
   <si>
-    <t>double separator</t>
-  </si>
-  <si>
-    <t>no separator</t>
-  </si>
-  <si>
     <t>gr_as_004</t>
   </si>
   <si>
@@ -138,9 +84,6 @@
     <t>gr_as_006</t>
   </si>
   <si>
-    <t>separator different than .</t>
-  </si>
-  <si>
     <t>row with abnormal length</t>
   </si>
   <si>
@@ -193,6 +136,114 @@
   </si>
   <si>
     <t>['Palabra AIRE encontrada entre (0, 0) y (3, 3).', 'Palabra AGUA encontrada entre (0, 0) y (0, 3).', 'Palabra TIERRA no encontrada.', 'Palabra NIU encontrada entre (2, 0) y (0, 2).']</t>
+  </si>
+  <si>
+    <t>double node 1</t>
+  </si>
+  <si>
+    <t>delete node 1</t>
+  </si>
+  <si>
+    <t>modify node 1</t>
+  </si>
+  <si>
+    <t>double node 2</t>
+  </si>
+  <si>
+    <t>delete node 2</t>
+  </si>
+  <si>
+    <t>double node 3</t>
+  </si>
+  <si>
+    <t>delete node 3</t>
+  </si>
+  <si>
+    <t>double node 4</t>
+  </si>
+  <si>
+    <t>delete node 4</t>
+  </si>
+  <si>
+    <t>modify node 5</t>
+  </si>
+  <si>
+    <t>modify node 6</t>
+  </si>
+  <si>
+    <t>modify node 7</t>
+  </si>
+  <si>
+    <t>gr_as_007</t>
+  </si>
+  <si>
+    <t>gr_as_008</t>
+  </si>
+  <si>
+    <t>gr_as_009</t>
+  </si>
+  <si>
+    <t>gr_as_010</t>
+  </si>
+  <si>
+    <t>gr_as_011</t>
+  </si>
+  <si>
+    <t>gr_as_012</t>
+  </si>
+  <si>
+    <t>double the content of a correct file</t>
+  </si>
+  <si>
+    <t>empty file</t>
+  </si>
+  <si>
+    <t>something that has nothing to do with the matter</t>
+  </si>
+  <si>
+    <t>no wordlist</t>
+  </si>
+  <si>
+    <t>Wordlist must contain at least one word.</t>
+  </si>
+  <si>
+    <t>wordlist repeated, actually there is nothing wrong with that</t>
+  </si>
+  <si>
+    <t>Incorrect format. No table found.</t>
+  </si>
+  <si>
+    <t>['Palabra AIRE encontrada entre (0, 0) y (3, 3).', 'Palabra AGUA encontrada entre (0, 0) y (0, 3).', 'Palabra TIERRA no encontrada.', 'Palabra NIU encontrada entre (2, 0) y (0, 2).', 'Palabra AIRE encontrada entre (0, 0) y (3, 3).', 'Palabra AGUA encontrada entre (0, 0) y (0, 3).', 'Palabra TIERRA no encontrada.', 'Palabra NIU encontrada entre (2, 0) y (0, 2).']</t>
+  </si>
+  <si>
+    <t>Symbols mixed with letters</t>
+  </si>
+  <si>
+    <t>ms_as_001</t>
+  </si>
+  <si>
+    <t>ms_as_002</t>
+  </si>
+  <si>
+    <t>ms_as_003</t>
+  </si>
+  <si>
+    <t>ms_as_004</t>
+  </si>
+  <si>
+    <t>Good test 1</t>
+  </si>
+  <si>
+    <t>Good test 2</t>
+  </si>
+  <si>
+    <t>Good test 3</t>
+  </si>
+  <si>
+    <t>Good test 4</t>
+  </si>
+  <si>
+    <t>['Palabra ABADESA encontrada entre (8, 6) y (2, 0).', 'Palabra BALANO encontrada entre (6, 1) y (6, 6).', 'Palabra BATERIA encontrada entre (7, 9) y (1, 9).', 'Palabra BORDADO encontrada entre (3, 12) y (9, 12).', 'Palabra CIERVA encontrada entre (3, 2) y (3, 7).', 'Palabra INTERNO encontrada entre (9, 3) y (9, 9).', 'Palabra LLUVIA encontrada entre (3, 0) y (8, 0).', 'Palabra MARTY encontrada entre (5, 10) y (1, 10).', 'Palabra MINIMO encontrada entre (0, 3) y (0, 8).', 'Palabra PAJIZO encontrada entre (2, 6) y (2, 1).', 'Palabra PAÑUELO encontrada entre (1, 8) y (7, 8).', 'Palabra SCHOTTE encontrada entre (7, 11) y (1, 11).', 'Palabra SOFIA encontrada entre (4, 3) y (4, 7).', 'Palabra SOLARIS encontrada entre (10, 4) y (10, 10).']</t>
   </si>
 </sst>
 </file>
@@ -604,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C766BE2E-A501-4A19-9656-5430AC1749FA}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,131 +673,131 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="2"/>
@@ -755,7 +806,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
@@ -766,258 +817,249 @@
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
tests added refactor in FileParser
</commit_message>
<xml_diff>
--- a/docs/tests_index.xlsx
+++ b/docs/tests_index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\repos\games\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58BCA60-2FDE-479D-9CBA-B37988417E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913A0A42-3A65-4D4F-8276-BBC45DEB7D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17592" windowHeight="11652" xr2:uid="{B783D0B5-C6EA-4FCF-B986-EFEDF66F7BFD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
   <si>
     <t>ce_as_001</t>
   </si>
@@ -135,9 +135,6 @@
     <t>non alphabetical characters in wordlist</t>
   </si>
   <si>
-    <t>['Palabra AIRE encontrada entre (0, 0) y (3, 3).', 'Palabra AGUA encontrada entre (0, 0) y (0, 3).', 'Palabra TIERRA no encontrada.', 'Palabra NIU encontrada entre (2, 0) y (0, 2).']</t>
-  </si>
-  <si>
     <t>double node 1</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>Incorrect format. No table found.</t>
   </si>
   <si>
-    <t>['Palabra AIRE encontrada entre (0, 0) y (3, 3).', 'Palabra AGUA encontrada entre (0, 0) y (0, 3).', 'Palabra TIERRA no encontrada.', 'Palabra NIU encontrada entre (2, 0) y (0, 2).', 'Palabra AIRE encontrada entre (0, 0) y (3, 3).', 'Palabra AGUA encontrada entre (0, 0) y (0, 3).', 'Palabra TIERRA no encontrada.', 'Palabra NIU encontrada entre (2, 0) y (0, 2).']</t>
-  </si>
-  <si>
     <t>Symbols mixed with letters</t>
   </si>
   <si>
@@ -237,13 +231,43 @@
     <t>Good test 2</t>
   </si>
   <si>
-    <t>Good test 3</t>
-  </si>
-  <si>
     <t>Good test 4</t>
   </si>
   <si>
-    <t>['Palabra ABADESA encontrada entre (8, 6) y (2, 0).', 'Palabra BALANO encontrada entre (6, 1) y (6, 6).', 'Palabra BATERIA encontrada entre (7, 9) y (1, 9).', 'Palabra BORDADO encontrada entre (3, 12) y (9, 12).', 'Palabra CIERVA encontrada entre (3, 2) y (3, 7).', 'Palabra INTERNO encontrada entre (9, 3) y (9, 9).', 'Palabra LLUVIA encontrada entre (3, 0) y (8, 0).', 'Palabra MARTY encontrada entre (5, 10) y (1, 10).', 'Palabra MINIMO encontrada entre (0, 3) y (0, 8).', 'Palabra PAJIZO encontrada entre (2, 6) y (2, 1).', 'Palabra PAÑUELO encontrada entre (1, 8) y (7, 8).', 'Palabra SCHOTTE encontrada entre (7, 11) y (1, 11).', 'Palabra SOFIA encontrada entre (4, 3) y (4, 7).', 'Palabra SOLARIS encontrada entre (10, 4) y (10, 10).']</t>
+    <t>['Palabra ABADESA encontrada entre (9, 7) y (3, 1).', 'Palabra BALANO encontrada entre (7, 2) y (7, 7).', 'Palabra BATERIA encontrada entre (8, 10) y (2, 10).', 'Palabra BORDADO encontrada entre (4, 13) y (10, 13).', 'Palabra CIERVA encontrada entre (4, 3) y (4, 8).', 'Palabra INTERNO encontrada entre (10, 4) y (10, 10).', 'Palabra LLUVIA encontrada entre (4, 1) y (9, 1).', 'Palabra MARTY encontrada entre (6, 11) y (2, 11).', 'Palabra MINIMO encontrada entre (1, 4) y (1, 9).', 'Palabra PAJIZO encontrada entre (3, 7) y (3, 2).', 'Palabra PAÑUELO encontrada entre (2, 9) y (8, 9).', 'Palabra SCHOTTE encontrada entre (8, 12) y (2, 12).', 'Palabra SOFIA encontrada entre (5, 4) y (5, 8).', 'Palabra SOLARIS encontrada entre (11, 5) y (11, 11).']</t>
+  </si>
+  <si>
+    <t>['Palabra AIRE encontrada entre (1, 1) y (4, 4).', 'Palabra AGUA encontrada entre (1, 1) y (1, 4).', 'Palabra TIERRA no encontrada.', 'Palabra NIU encontrada entre (3, 1) y (1, 3).']</t>
+  </si>
+  <si>
+    <t>['Palabra ADOPCION encontrada entre (22, 2) y (22, 9).', 'Palabra ADORNO encontrada entre (8, 4) y (13, 9).', 'Palabra ALHAJA encontrada entre (23, 1) y (28, 6).', 'Palabra ALIANZA encontrada entre (6, 9) y (12, 9).', 'Palabra AMOR encontrada entre (18, 6) y (18, 9).', 'Palabra ANILLO encontrada entre (10, 1) y (15, 6).', 'Palabra BONDAD encontrada entre (1, 8) y (6, 3).', 'Palabra CALMA encontrada entre (18, 5) y (14, 1).', 'Palabra CANDOR encontrada entre (20, 13) y (25, 8).', 'Palabra CARIÑOS encontrada entre (13, 3) y (19, 9).', 'Palabra DIADEMA encontrada entre (4, 2) y (10, 2).', 'Palabra ESTILO encontrada entre (10, 3) y (5, 8).', 'Palabra ETICA encontrada entre (2, 9) y (6, 9).', 'Palabra FIESTA encontrada entre (23, 8) y (28, 3).', 'Palabra FORTUNA encontrada entre (22, 13) y (28, 13).', 'Palabra GEMA encontrada entre (20, 7) y (20, 10).', 'Palabra GOZO encontrada entre (20, 6) y (20, 3).', 'Palabra HUMILDAD encontrada entre (11, 3) y (18, 10).', 'Palabra LEALTAD encontrada entre (27, 6) y (27, 12).', 'Palabra MAJESTAD encontrada entre (12, 11) y (19, 11).', 'Palabra MESURA encontrada entre (4, 11) y (9, 11).', 'Palabra MODESTIA encontrada entre (21, 1) y (21, 8).', 'Palabra MUSICA encontrada entre (12, 11) y (17, 6).', 'Palabra NACAR encontrada entre (28, 5) y (28, 9).', 'Palabra PERDON encontrada entre (3, 10) y (8, 10).', 'Palabra PLATINO encontrada entre (2, 12) y (8, 12).', 'Palabra PREMIO encontrada entre (15, 10) y (20, 5).', 'Palabra PUREZA encontrada entre (9, 3) y (14, 8).', 'Palabra RECREO encontrada entre (3, 11) y (8, 6).', 'Palabra RISA encontrada entre (15, 1) y (18, 4).', 'Palabra SANTIDAD encontrada entre (19, 13) y (26, 6).', 'Palabra SORTIJA encontrada entre (9, 13) y (3, 13).', 'Palabra TACTO encontrada entre (2, 1) y (6, 1).', 'Palabra TEATRO encontrada entre (26, 7) y (26, 12).', 'Palabra VIRTUD encontrada entre (1, 9) y (6, 4).']</t>
+  </si>
+  <si>
+    <t>Bad test 1</t>
+  </si>
+  <si>
+    <t>gr_as_013</t>
+  </si>
+  <si>
+    <t>gr_as_014</t>
+  </si>
+  <si>
+    <t>word out of bounds horizontally</t>
+  </si>
+  <si>
+    <t>['Palabra PAJARO no encontrada.', 'Palabra PASA encontrada entre (1, 1) y (1, 4).']</t>
+  </si>
+  <si>
+    <t>Word PAJARO couldn't be found as it is splitted (see test file)</t>
+  </si>
+  <si>
+    <t>word out of bounds vertically</t>
+  </si>
+  <si>
+    <t>gr_as_015</t>
+  </si>
+  <si>
+    <t>Word PAJARO couldn't be found as it gets out of the table</t>
   </si>
 </sst>
 </file>
@@ -655,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C766BE2E-A501-4A19-9656-5430AC1749FA}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,7 +723,7 @@
         <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -821,13 +845,13 @@
         <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -838,13 +862,13 @@
         <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -855,13 +879,13 @@
         <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -872,13 +896,13 @@
         <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>59</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -889,13 +913,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -906,7 +930,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>30</v>
@@ -915,13 +939,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>30</v>
@@ -930,60 +954,60 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>30</v>
@@ -992,74 +1016,127 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>